<commit_message>
Modificación de  evaluación "aparece en el cuaderno"
Modificación de  evaluación "aparece en el cuaderno"
</commit_message>
<xml_diff>
--- a/fuentes/contenidos/grado10/guion09/ESCALETA FINAL CN_10_09.xlsx
+++ b/fuentes/contenidos/grado10/guion09/ESCALETA FINAL CN_10_09.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LyzMarcela\Desktop\Edición Planeta\CN_10_09_CO\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LyzMarcela\Documents\GitHub\CienciasNaturales\fuentes\contenidos\grado10\guion09\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -655,9 +655,6 @@
     <t>Recurso F6-01</t>
   </si>
   <si>
-    <t xml:space="preserve">La energía cinética y potencial </t>
-  </si>
-  <si>
     <t>http://hispanicasaber.planetasaber.com/encyclopedia/default.asp?idpack=5&amp;idpil=AN001193&amp;ruta=Buscador</t>
   </si>
   <si>
@@ -764,6 +761,9 @@
   </si>
   <si>
     <t xml:space="preserve"> Motor que incluye preguntas de respuesta abierta del tema La materia y la energía</t>
+  </si>
+  <si>
+    <t>Identifica la energía cinética y la potencial</t>
   </si>
 </sst>
 </file>
@@ -1026,34 +1026,19 @@
     <xf numFmtId="0" fontId="4" fillId="12" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1098,8 +1083,23 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1408,9 +1408,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U292"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E12" sqref="E12"/>
+    <sheetView tabSelected="1" topLeftCell="J1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A26" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="P38" sqref="P38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1438,94 +1438,94 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" s="23" customFormat="1" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="41" t="s">
+      <c r="A1" s="36" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="39" t="s">
+      <c r="B1" s="34" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="51" t="s">
+      <c r="C1" s="46" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="41" t="s">
+      <c r="D1" s="36" t="s">
         <v>111</v>
       </c>
-      <c r="E1" s="39" t="s">
+      <c r="E1" s="34" t="s">
         <v>112</v>
       </c>
-      <c r="F1" s="37" t="s">
+      <c r="F1" s="30" t="s">
         <v>113</v>
       </c>
-      <c r="G1" s="43" t="s">
+      <c r="G1" s="38" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="37" t="s">
+      <c r="H1" s="30" t="s">
         <v>114</v>
       </c>
-      <c r="I1" s="37" t="s">
+      <c r="I1" s="30" t="s">
         <v>108</v>
       </c>
-      <c r="J1" s="47" t="s">
+      <c r="J1" s="42" t="s">
         <v>4</v>
       </c>
-      <c r="K1" s="45" t="s">
+      <c r="K1" s="40" t="s">
         <v>109</v>
       </c>
-      <c r="L1" s="43" t="s">
+      <c r="L1" s="38" t="s">
         <v>14</v>
       </c>
-      <c r="M1" s="49" t="s">
+      <c r="M1" s="44" t="s">
         <v>21</v>
       </c>
-      <c r="N1" s="49"/>
-      <c r="O1" s="29" t="s">
+      <c r="N1" s="44"/>
+      <c r="O1" s="32" t="s">
         <v>110</v>
       </c>
-      <c r="P1" s="29" t="s">
+      <c r="P1" s="32" t="s">
         <v>115</v>
       </c>
-      <c r="Q1" s="31" t="s">
+      <c r="Q1" s="48" t="s">
         <v>86</v>
       </c>
-      <c r="R1" s="35" t="s">
+      <c r="R1" s="52" t="s">
         <v>87</v>
       </c>
-      <c r="S1" s="31" t="s">
+      <c r="S1" s="48" t="s">
         <v>88</v>
       </c>
-      <c r="T1" s="33" t="s">
+      <c r="T1" s="50" t="s">
         <v>89</v>
       </c>
-      <c r="U1" s="31" t="s">
+      <c r="U1" s="48" t="s">
         <v>90</v>
       </c>
     </row>
     <row r="2" spans="1:21" s="23" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="42"/>
-      <c r="B2" s="40"/>
-      <c r="C2" s="52"/>
-      <c r="D2" s="42"/>
-      <c r="E2" s="40"/>
-      <c r="F2" s="38"/>
-      <c r="G2" s="50"/>
-      <c r="H2" s="38"/>
-      <c r="I2" s="38"/>
-      <c r="J2" s="48"/>
-      <c r="K2" s="46"/>
-      <c r="L2" s="44"/>
+      <c r="A2" s="37"/>
+      <c r="B2" s="35"/>
+      <c r="C2" s="47"/>
+      <c r="D2" s="37"/>
+      <c r="E2" s="35"/>
+      <c r="F2" s="31"/>
+      <c r="G2" s="45"/>
+      <c r="H2" s="31"/>
+      <c r="I2" s="31"/>
+      <c r="J2" s="43"/>
+      <c r="K2" s="41"/>
+      <c r="L2" s="39"/>
       <c r="M2" s="24" t="s">
         <v>91</v>
       </c>
       <c r="N2" s="24" t="s">
         <v>92</v>
       </c>
-      <c r="O2" s="30"/>
-      <c r="P2" s="30"/>
-      <c r="Q2" s="32"/>
-      <c r="R2" s="36"/>
-      <c r="S2" s="32"/>
-      <c r="T2" s="34"/>
-      <c r="U2" s="32"/>
+      <c r="O2" s="33"/>
+      <c r="P2" s="33"/>
+      <c r="Q2" s="49"/>
+      <c r="R2" s="53"/>
+      <c r="S2" s="49"/>
+      <c r="T2" s="51"/>
+      <c r="U2" s="49"/>
     </row>
     <row r="3" spans="1:21" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
@@ -1646,7 +1646,7 @@
         <v>20</v>
       </c>
       <c r="J5" s="17" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="K5" s="7" t="s">
         <v>20</v>
@@ -1768,7 +1768,7 @@
         <v>20</v>
       </c>
       <c r="J7" s="27" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="K7" s="7" t="s">
         <v>20</v>
@@ -2558,7 +2558,7 @@
         <v>146</v>
       </c>
       <c r="G22" s="16" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="H22" s="18">
         <v>15</v>
@@ -2567,7 +2567,7 @@
         <v>20</v>
       </c>
       <c r="J22" s="17" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="K22" s="7" t="s">
         <v>20</v>
@@ -2593,7 +2593,7 @@
         <v>164</v>
       </c>
       <c r="T22" s="12" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="U22" s="10" t="s">
         <v>166</v>
@@ -2626,7 +2626,7 @@
         <v>20</v>
       </c>
       <c r="J23" s="17" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="K23" s="7" t="s">
         <v>20</v>
@@ -2652,7 +2652,7 @@
         <v>164</v>
       </c>
       <c r="T23" s="12" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="U23" s="10" t="s">
         <v>166</v>
@@ -2735,7 +2735,7 @@
       </c>
       <c r="F25" s="9"/>
       <c r="G25" s="16" t="s">
-        <v>209</v>
+        <v>245</v>
       </c>
       <c r="H25" s="18">
         <v>18</v>
@@ -2744,7 +2744,7 @@
         <v>20</v>
       </c>
       <c r="J25" s="27" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="K25" s="7" t="s">
         <v>20</v>
@@ -2757,7 +2757,7 @@
         <v>34</v>
       </c>
       <c r="O25" s="28" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="P25" s="9" t="s">
         <v>19</v>
@@ -2772,7 +2772,7 @@
         <v>164</v>
       </c>
       <c r="T25" s="12" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="U25" s="10" t="s">
         <v>166</v>
@@ -2796,7 +2796,7 @@
       </c>
       <c r="F26" s="9"/>
       <c r="G26" s="16" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="H26" s="18">
         <v>19</v>
@@ -2805,7 +2805,7 @@
         <v>20</v>
       </c>
       <c r="J26" s="27" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="K26" s="7" t="s">
         <v>20</v>
@@ -2831,7 +2831,7 @@
         <v>164</v>
       </c>
       <c r="T26" s="12" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="U26" s="10" t="s">
         <v>166</v>
@@ -2892,7 +2892,7 @@
         <v>148</v>
       </c>
       <c r="G28" s="16" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="H28" s="18">
         <v>20</v>
@@ -2901,7 +2901,7 @@
         <v>20</v>
       </c>
       <c r="J28" s="27" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="K28" s="7" t="s">
         <v>20</v>
@@ -2914,7 +2914,7 @@
         <v>34</v>
       </c>
       <c r="O28" s="28" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="P28" s="9" t="s">
         <v>19</v>
@@ -2929,7 +2929,7 @@
         <v>164</v>
       </c>
       <c r="T28" s="12" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="U28" s="10" t="s">
         <v>166</v>
@@ -3012,7 +3012,7 @@
       </c>
       <c r="F30" s="9"/>
       <c r="G30" s="16" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="H30" s="18">
         <v>22</v>
@@ -3021,7 +3021,7 @@
         <v>20</v>
       </c>
       <c r="J30" s="27" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="K30" s="7" t="s">
         <v>20</v>
@@ -3047,7 +3047,7 @@
         <v>164</v>
       </c>
       <c r="T30" s="12" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="U30" s="10" t="s">
         <v>166</v>
@@ -3080,7 +3080,7 @@
         <v>20</v>
       </c>
       <c r="J31" s="17" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="K31" s="7" t="s">
         <v>20</v>
@@ -3106,7 +3106,7 @@
         <v>164</v>
       </c>
       <c r="T31" s="12" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="U31" s="10" t="s">
         <v>166</v>
@@ -3127,8 +3127,8 @@
       </c>
       <c r="E32" s="13"/>
       <c r="F32" s="9"/>
-      <c r="G32" s="53" t="s">
-        <v>240</v>
+      <c r="G32" s="29" t="s">
+        <v>239</v>
       </c>
       <c r="H32" s="18">
         <v>24</v>
@@ -3137,7 +3137,7 @@
         <v>20</v>
       </c>
       <c r="J32" s="27" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="K32" s="7" t="s">
         <v>20</v>
@@ -3163,7 +3163,7 @@
         <v>164</v>
       </c>
       <c r="T32" s="12" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="U32" s="10" t="s">
         <v>166</v>
@@ -3184,8 +3184,8 @@
       </c>
       <c r="E33" s="13"/>
       <c r="F33" s="9"/>
-      <c r="G33" s="53" t="s">
-        <v>234</v>
+      <c r="G33" s="29" t="s">
+        <v>233</v>
       </c>
       <c r="H33" s="18">
         <v>25</v>
@@ -3194,7 +3194,7 @@
         <v>20</v>
       </c>
       <c r="J33" s="27" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="K33" s="7" t="s">
         <v>20</v>
@@ -3220,7 +3220,7 @@
         <v>164</v>
       </c>
       <c r="T33" s="12" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="U33" s="10" t="s">
         <v>166</v>
@@ -3237,7 +3237,7 @@
         <v>123</v>
       </c>
       <c r="D34" s="15" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="E34" s="13"/>
       <c r="F34" s="9"/>
@@ -3251,7 +3251,7 @@
         <v>20</v>
       </c>
       <c r="J34" s="17" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="K34" s="7" t="s">
         <v>20</v>
@@ -3280,12 +3280,12 @@
         <v>123</v>
       </c>
       <c r="D35" s="15" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="E35" s="13"/>
       <c r="F35" s="9"/>
       <c r="G35" s="16" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="H35" s="18">
         <v>27</v>
@@ -3294,7 +3294,7 @@
         <v>20</v>
       </c>
       <c r="J35" s="17" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="K35" s="7" t="s">
         <v>20</v>
@@ -3308,7 +3308,7 @@
       </c>
       <c r="O35" s="9"/>
       <c r="P35" s="9" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="Q35" s="10">
         <v>6</v>
@@ -3320,7 +3320,7 @@
         <v>164</v>
       </c>
       <c r="T35" s="12" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="U35" s="10" t="s">
         <v>166</v>
@@ -3340,7 +3340,7 @@
       <c r="E36" s="13"/>
       <c r="F36" s="9"/>
       <c r="G36" s="16" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="H36" s="18">
         <v>28</v>
@@ -3349,7 +3349,7 @@
         <v>20</v>
       </c>
       <c r="J36" s="17" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="K36" s="7" t="s">
         <v>20</v>
@@ -3375,7 +3375,7 @@
         <v>164</v>
       </c>
       <c r="T36" s="12" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="U36" s="10" t="s">
         <v>166</v>
@@ -4713,6 +4713,12 @@
     <filterColumn colId="12" showButton="0"/>
   </autoFilter>
   <mergeCells count="20">
+    <mergeCell ref="P1:P2"/>
+    <mergeCell ref="U1:U2"/>
+    <mergeCell ref="T1:T2"/>
+    <mergeCell ref="S1:S2"/>
+    <mergeCell ref="R1:R2"/>
+    <mergeCell ref="Q1:Q2"/>
     <mergeCell ref="I1:I2"/>
     <mergeCell ref="H1:H2"/>
     <mergeCell ref="O1:O2"/>
@@ -4727,12 +4733,6 @@
     <mergeCell ref="D1:D2"/>
     <mergeCell ref="C1:C2"/>
     <mergeCell ref="F1:F2"/>
-    <mergeCell ref="P1:P2"/>
-    <mergeCell ref="U1:U2"/>
-    <mergeCell ref="T1:T2"/>
-    <mergeCell ref="S1:S2"/>
-    <mergeCell ref="R1:R2"/>
-    <mergeCell ref="Q1:Q2"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="O21" r:id="rId1"/>

</xml_diff>

<commit_message>
Complementar información aparece cuaderno de estudio
Complementar información aparece cuaderno de estudio
</commit_message>
<xml_diff>
--- a/fuentes/contenidos/grado10/guion09/ESCALETA FINAL CN_10_09.xlsx
+++ b/fuentes/contenidos/grado10/guion09/ESCALETA FINAL CN_10_09.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="604" uniqueCount="246">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="605" uniqueCount="246">
   <si>
     <t>Asignatura</t>
   </si>
@@ -1029,16 +1029,34 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1081,24 +1099,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1408,9 +1408,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U292"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A26" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="P38" sqref="P38"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A18" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="P34" sqref="P34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1438,94 +1438,94 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" s="23" customFormat="1" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="36" t="s">
+      <c r="A1" s="42" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="34" t="s">
+      <c r="B1" s="40" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="46" t="s">
+      <c r="C1" s="52" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="36" t="s">
+      <c r="D1" s="42" t="s">
         <v>111</v>
       </c>
-      <c r="E1" s="34" t="s">
+      <c r="E1" s="40" t="s">
         <v>112</v>
       </c>
-      <c r="F1" s="30" t="s">
+      <c r="F1" s="38" t="s">
         <v>113</v>
       </c>
-      <c r="G1" s="38" t="s">
+      <c r="G1" s="44" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="30" t="s">
+      <c r="H1" s="38" t="s">
         <v>114</v>
       </c>
-      <c r="I1" s="30" t="s">
+      <c r="I1" s="38" t="s">
         <v>108</v>
       </c>
-      <c r="J1" s="42" t="s">
+      <c r="J1" s="48" t="s">
         <v>4</v>
       </c>
-      <c r="K1" s="40" t="s">
+      <c r="K1" s="46" t="s">
         <v>109</v>
       </c>
-      <c r="L1" s="38" t="s">
+      <c r="L1" s="44" t="s">
         <v>14</v>
       </c>
-      <c r="M1" s="44" t="s">
+      <c r="M1" s="50" t="s">
         <v>21</v>
       </c>
-      <c r="N1" s="44"/>
-      <c r="O1" s="32" t="s">
+      <c r="N1" s="50"/>
+      <c r="O1" s="30" t="s">
         <v>110</v>
       </c>
-      <c r="P1" s="32" t="s">
+      <c r="P1" s="30" t="s">
         <v>115</v>
       </c>
-      <c r="Q1" s="48" t="s">
+      <c r="Q1" s="32" t="s">
         <v>86</v>
       </c>
-      <c r="R1" s="52" t="s">
+      <c r="R1" s="36" t="s">
         <v>87</v>
       </c>
-      <c r="S1" s="48" t="s">
+      <c r="S1" s="32" t="s">
         <v>88</v>
       </c>
-      <c r="T1" s="50" t="s">
+      <c r="T1" s="34" t="s">
         <v>89</v>
       </c>
-      <c r="U1" s="48" t="s">
+      <c r="U1" s="32" t="s">
         <v>90</v>
       </c>
     </row>
     <row r="2" spans="1:21" s="23" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="37"/>
-      <c r="B2" s="35"/>
-      <c r="C2" s="47"/>
-      <c r="D2" s="37"/>
-      <c r="E2" s="35"/>
-      <c r="F2" s="31"/>
-      <c r="G2" s="45"/>
-      <c r="H2" s="31"/>
-      <c r="I2" s="31"/>
-      <c r="J2" s="43"/>
-      <c r="K2" s="41"/>
-      <c r="L2" s="39"/>
+      <c r="A2" s="43"/>
+      <c r="B2" s="41"/>
+      <c r="C2" s="53"/>
+      <c r="D2" s="43"/>
+      <c r="E2" s="41"/>
+      <c r="F2" s="39"/>
+      <c r="G2" s="51"/>
+      <c r="H2" s="39"/>
+      <c r="I2" s="39"/>
+      <c r="J2" s="49"/>
+      <c r="K2" s="47"/>
+      <c r="L2" s="45"/>
       <c r="M2" s="24" t="s">
         <v>91</v>
       </c>
       <c r="N2" s="24" t="s">
         <v>92</v>
       </c>
-      <c r="O2" s="33"/>
-      <c r="P2" s="33"/>
-      <c r="Q2" s="49"/>
-      <c r="R2" s="53"/>
-      <c r="S2" s="49"/>
-      <c r="T2" s="51"/>
-      <c r="U2" s="49"/>
+      <c r="O2" s="31"/>
+      <c r="P2" s="31"/>
+      <c r="Q2" s="33"/>
+      <c r="R2" s="37"/>
+      <c r="S2" s="33"/>
+      <c r="T2" s="35"/>
+      <c r="U2" s="33"/>
     </row>
     <row r="3" spans="1:21" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
@@ -3262,7 +3262,9 @@
       <c r="M34" s="8"/>
       <c r="N34" s="8"/>
       <c r="O34" s="9"/>
-      <c r="P34" s="9"/>
+      <c r="P34" s="9" t="s">
+        <v>19</v>
+      </c>
       <c r="Q34" s="10"/>
       <c r="R34" s="11"/>
       <c r="S34" s="10"/>
@@ -4713,12 +4715,6 @@
     <filterColumn colId="12" showButton="0"/>
   </autoFilter>
   <mergeCells count="20">
-    <mergeCell ref="P1:P2"/>
-    <mergeCell ref="U1:U2"/>
-    <mergeCell ref="T1:T2"/>
-    <mergeCell ref="S1:S2"/>
-    <mergeCell ref="R1:R2"/>
-    <mergeCell ref="Q1:Q2"/>
     <mergeCell ref="I1:I2"/>
     <mergeCell ref="H1:H2"/>
     <mergeCell ref="O1:O2"/>
@@ -4733,6 +4729,12 @@
     <mergeCell ref="D1:D2"/>
     <mergeCell ref="C1:C2"/>
     <mergeCell ref="F1:F2"/>
+    <mergeCell ref="P1:P2"/>
+    <mergeCell ref="U1:U2"/>
+    <mergeCell ref="T1:T2"/>
+    <mergeCell ref="S1:S2"/>
+    <mergeCell ref="R1:R2"/>
+    <mergeCell ref="Q1:Q2"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="O21" r:id="rId1"/>

</xml_diff>

<commit_message>
Cambio de lugar de recursos
Cambio de lugar de recursos
</commit_message>
<xml_diff>
--- a/fuentes/contenidos/grado10/guion09/ESCALETA FINAL CN_10_09.xlsx
+++ b/fuentes/contenidos/grado10/guion09/ESCALETA FINAL CN_10_09.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LyzMarcela\Documents\GitHub\CienciasNaturales\fuentes\contenidos\grado10\guion09\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LyzMarcela\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -16,14 +16,14 @@
     <sheet name="DATOS" sheetId="1" state="hidden" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Hoja2!$A$1:$U$32</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Hoja2!$A$1:$U$36</definedName>
   </definedNames>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="605" uniqueCount="246">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="600" uniqueCount="248">
   <si>
     <t>Asignatura</t>
   </si>
@@ -481,9 +481,6 @@
     <t xml:space="preserve">Refuerza tu aprendizaje: Las transformaciones de la materia </t>
   </si>
   <si>
-    <t>Las técnicas de separación de mezclas</t>
-  </si>
-  <si>
     <t>Refuerza tu aprendizaje: La clasificación de la materia</t>
   </si>
   <si>
@@ -532,9 +529,6 @@
     <t>Recurso M101A-01</t>
   </si>
   <si>
-    <t>Recurso F12-01</t>
-  </si>
-  <si>
     <t>Recurso M101A-02</t>
   </si>
   <si>
@@ -556,9 +550,6 @@
     <t>Los estados y las transformaciones físicas</t>
   </si>
   <si>
-    <t xml:space="preserve">Interactivo con animación incluida que permite explicar los diferentes estados de la materia y sus transformaciones físicas </t>
-  </si>
-  <si>
     <t>Identifica las transformaciones físicas</t>
   </si>
   <si>
@@ -574,18 +565,9 @@
     <t xml:space="preserve">Actividades sobre  Las transformaciones de la materia </t>
   </si>
   <si>
-    <t xml:space="preserve">Los elementos y los compuestos </t>
-  </si>
-  <si>
-    <t>Secuencia de imágenes que permiten exponer las diferencias entre elemento y compuesto</t>
-  </si>
-  <si>
     <t>Recursos M aleatorios y diaporama F1</t>
   </si>
   <si>
-    <t>Diaporama F1-01</t>
-  </si>
-  <si>
     <t>RM_01_02_CO</t>
   </si>
   <si>
@@ -646,9 +628,6 @@
     <t>Diaporama F1-02</t>
   </si>
   <si>
-    <t>Las temperatura</t>
-  </si>
-  <si>
     <t xml:space="preserve">Interactivo que muestra las diferentes escalas de temperatura y las conversiones  </t>
   </si>
   <si>
@@ -764,6 +743,33 @@
   </si>
   <si>
     <t>Identifica la energía cinética y la potencial</t>
+  </si>
+  <si>
+    <t>Recursos adicionales 01</t>
+  </si>
+  <si>
+    <t>Video como media principal - 01</t>
+  </si>
+  <si>
+    <t>RF_01_02_CO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Animación que permite explicar los diferentes estados de la materia y sus transformaciones físicas </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Las sustancias puras y las mezclas </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Interactivo que permiten exponer las diferencias entre las sustancias puras y las mezclas </t>
+  </si>
+  <si>
+    <t>Recurso F7-03</t>
+  </si>
+  <si>
+    <t>La separación de mezclas</t>
+  </si>
+  <si>
+    <t>La temperatura</t>
   </si>
 </sst>
 </file>
@@ -1029,34 +1035,16 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1099,6 +1087,24 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1408,9 +1414,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U292"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A18" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="P34" sqref="P34"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A24" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G32" sqref="G32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1438,94 +1444,94 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" s="23" customFormat="1" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="42" t="s">
+      <c r="A1" s="36" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="40" t="s">
+      <c r="B1" s="34" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="52" t="s">
+      <c r="C1" s="46" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="42" t="s">
+      <c r="D1" s="36" t="s">
         <v>111</v>
       </c>
-      <c r="E1" s="40" t="s">
+      <c r="E1" s="34" t="s">
         <v>112</v>
       </c>
-      <c r="F1" s="38" t="s">
+      <c r="F1" s="30" t="s">
         <v>113</v>
       </c>
-      <c r="G1" s="44" t="s">
+      <c r="G1" s="38" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="38" t="s">
+      <c r="H1" s="30" t="s">
         <v>114</v>
       </c>
-      <c r="I1" s="38" t="s">
+      <c r="I1" s="30" t="s">
         <v>108</v>
       </c>
-      <c r="J1" s="48" t="s">
+      <c r="J1" s="42" t="s">
         <v>4</v>
       </c>
-      <c r="K1" s="46" t="s">
+      <c r="K1" s="40" t="s">
         <v>109</v>
       </c>
-      <c r="L1" s="44" t="s">
+      <c r="L1" s="38" t="s">
         <v>14</v>
       </c>
-      <c r="M1" s="50" t="s">
+      <c r="M1" s="44" t="s">
         <v>21</v>
       </c>
-      <c r="N1" s="50"/>
-      <c r="O1" s="30" t="s">
+      <c r="N1" s="44"/>
+      <c r="O1" s="32" t="s">
         <v>110</v>
       </c>
-      <c r="P1" s="30" t="s">
+      <c r="P1" s="32" t="s">
         <v>115</v>
       </c>
-      <c r="Q1" s="32" t="s">
+      <c r="Q1" s="48" t="s">
         <v>86</v>
       </c>
-      <c r="R1" s="36" t="s">
+      <c r="R1" s="52" t="s">
         <v>87</v>
       </c>
-      <c r="S1" s="32" t="s">
+      <c r="S1" s="48" t="s">
         <v>88</v>
       </c>
-      <c r="T1" s="34" t="s">
+      <c r="T1" s="50" t="s">
         <v>89</v>
       </c>
-      <c r="U1" s="32" t="s">
+      <c r="U1" s="48" t="s">
         <v>90</v>
       </c>
     </row>
     <row r="2" spans="1:21" s="23" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="43"/>
-      <c r="B2" s="41"/>
-      <c r="C2" s="53"/>
-      <c r="D2" s="43"/>
-      <c r="E2" s="41"/>
-      <c r="F2" s="39"/>
-      <c r="G2" s="51"/>
-      <c r="H2" s="39"/>
-      <c r="I2" s="39"/>
-      <c r="J2" s="49"/>
-      <c r="K2" s="47"/>
-      <c r="L2" s="45"/>
+      <c r="A2" s="37"/>
+      <c r="B2" s="35"/>
+      <c r="C2" s="47"/>
+      <c r="D2" s="37"/>
+      <c r="E2" s="35"/>
+      <c r="F2" s="31"/>
+      <c r="G2" s="45"/>
+      <c r="H2" s="31"/>
+      <c r="I2" s="31"/>
+      <c r="J2" s="43"/>
+      <c r="K2" s="41"/>
+      <c r="L2" s="39"/>
       <c r="M2" s="24" t="s">
         <v>91</v>
       </c>
       <c r="N2" s="24" t="s">
         <v>92</v>
       </c>
-      <c r="O2" s="31"/>
-      <c r="P2" s="31"/>
-      <c r="Q2" s="33"/>
-      <c r="R2" s="37"/>
-      <c r="S2" s="33"/>
-      <c r="T2" s="35"/>
-      <c r="U2" s="33"/>
+      <c r="O2" s="33"/>
+      <c r="P2" s="33"/>
+      <c r="Q2" s="49"/>
+      <c r="R2" s="53"/>
+      <c r="S2" s="49"/>
+      <c r="T2" s="51"/>
+      <c r="U2" s="49"/>
     </row>
     <row r="3" spans="1:21" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
@@ -1543,7 +1549,7 @@
       <c r="E3" s="13"/>
       <c r="F3" s="5"/>
       <c r="G3" s="16" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="H3" s="18">
         <v>1</v>
@@ -1552,7 +1558,7 @@
         <v>19</v>
       </c>
       <c r="J3" s="27" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="K3" s="20" t="s">
         <v>20</v>
@@ -1572,16 +1578,16 @@
         <v>6</v>
       </c>
       <c r="R3" s="11" t="s">
+        <v>158</v>
+      </c>
+      <c r="S3" s="10" t="s">
         <v>159</v>
       </c>
-      <c r="S3" s="10" t="s">
+      <c r="T3" s="12" t="s">
         <v>160</v>
       </c>
-      <c r="T3" s="12" t="s">
+      <c r="U3" s="10" t="s">
         <v>161</v>
-      </c>
-      <c r="U3" s="10" t="s">
-        <v>162</v>
       </c>
     </row>
     <row r="4" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
@@ -1637,7 +1643,7 @@
         <v>142</v>
       </c>
       <c r="G5" s="16" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="H5" s="18">
         <v>2</v>
@@ -1646,7 +1652,7 @@
         <v>20</v>
       </c>
       <c r="J5" s="17" t="s">
-        <v>228</v>
+        <v>221</v>
       </c>
       <c r="K5" s="7" t="s">
         <v>20</v>
@@ -1666,16 +1672,16 @@
         <v>6</v>
       </c>
       <c r="R5" s="11" t="s">
+        <v>162</v>
+      </c>
+      <c r="S5" s="10" t="s">
         <v>163</v>
       </c>
-      <c r="S5" s="10" t="s">
-        <v>164</v>
-      </c>
       <c r="T5" s="12" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="U5" s="10" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="6" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
@@ -1698,7 +1704,7 @@
         <v>142</v>
       </c>
       <c r="G6" s="16" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="H6" s="18">
         <v>3</v>
@@ -1707,7 +1713,7 @@
         <v>20</v>
       </c>
       <c r="J6" s="17" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="K6" s="7" t="s">
         <v>20</v>
@@ -1727,16 +1733,16 @@
         <v>6</v>
       </c>
       <c r="R6" s="11" t="s">
+        <v>162</v>
+      </c>
+      <c r="S6" s="10" t="s">
         <v>163</v>
       </c>
-      <c r="S6" s="10" t="s">
+      <c r="T6" s="12" t="s">
         <v>164</v>
       </c>
-      <c r="T6" s="12" t="s">
+      <c r="U6" s="10" t="s">
         <v>165</v>
-      </c>
-      <c r="U6" s="10" t="s">
-        <v>166</v>
       </c>
     </row>
     <row r="7" spans="1:21" ht="45" x14ac:dyDescent="0.25">
@@ -1759,7 +1765,7 @@
         <v>142</v>
       </c>
       <c r="G7" s="16" t="s">
-        <v>199</v>
+        <v>193</v>
       </c>
       <c r="H7" s="18">
         <v>4</v>
@@ -1768,7 +1774,7 @@
         <v>20</v>
       </c>
       <c r="J7" s="27" t="s">
-        <v>229</v>
+        <v>222</v>
       </c>
       <c r="K7" s="7" t="s">
         <v>20</v>
@@ -1781,7 +1787,7 @@
         <v>34</v>
       </c>
       <c r="O7" s="28" t="s">
-        <v>198</v>
+        <v>192</v>
       </c>
       <c r="P7" s="9" t="s">
         <v>19</v>
@@ -1790,16 +1796,16 @@
         <v>6</v>
       </c>
       <c r="R7" s="11" t="s">
+        <v>162</v>
+      </c>
+      <c r="S7" s="10" t="s">
         <v>163</v>
       </c>
-      <c r="S7" s="10" t="s">
-        <v>164</v>
-      </c>
       <c r="T7" s="12" t="s">
-        <v>190</v>
+        <v>184</v>
       </c>
       <c r="U7" s="10" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="8" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
@@ -1822,7 +1828,7 @@
         <v>143</v>
       </c>
       <c r="G8" s="16" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="H8" s="18">
         <v>5</v>
@@ -1831,7 +1837,7 @@
         <v>20</v>
       </c>
       <c r="J8" s="17" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="K8" s="7" t="s">
         <v>20</v>
@@ -1848,19 +1854,19 @@
         <v>20</v>
       </c>
       <c r="Q8" s="10" t="s">
-        <v>202</v>
+        <v>196</v>
       </c>
       <c r="R8" s="11" t="s">
+        <v>162</v>
+      </c>
+      <c r="S8" s="10" t="s">
         <v>163</v>
       </c>
-      <c r="S8" s="10" t="s">
-        <v>164</v>
-      </c>
       <c r="T8" s="12" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="U8" s="10" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="9" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
@@ -1890,7 +1896,7 @@
         <v>20</v>
       </c>
       <c r="J9" s="17" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="K9" s="7" t="s">
         <v>20</v>
@@ -1910,16 +1916,16 @@
         <v>6</v>
       </c>
       <c r="R9" s="11" t="s">
+        <v>162</v>
+      </c>
+      <c r="S9" s="10" t="s">
         <v>163</v>
       </c>
-      <c r="S9" s="10" t="s">
-        <v>164</v>
-      </c>
       <c r="T9" s="12" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="U9" s="10" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="10" spans="1:21" ht="49.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -1940,7 +1946,7 @@
       </c>
       <c r="F10" s="9"/>
       <c r="G10" s="16" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="H10" s="18">
         <v>7</v>
@@ -1949,7 +1955,7 @@
         <v>19</v>
       </c>
       <c r="J10" s="27" t="s">
-        <v>176</v>
+        <v>242</v>
       </c>
       <c r="K10" s="7" t="s">
         <v>20</v>
@@ -1957,12 +1963,10 @@
       <c r="L10" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="M10" s="8" t="s">
-        <v>63</v>
-      </c>
+      <c r="M10" s="8"/>
       <c r="N10" s="8"/>
       <c r="O10" s="28" t="s">
-        <v>197</v>
+        <v>191</v>
       </c>
       <c r="P10" s="9" t="s">
         <v>19</v>
@@ -1971,16 +1975,16 @@
         <v>6</v>
       </c>
       <c r="R10" s="11" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="S10" s="10" t="s">
-        <v>160</v>
+        <v>239</v>
       </c>
       <c r="T10" s="12" t="s">
-        <v>168</v>
+        <v>240</v>
       </c>
       <c r="U10" s="10" t="s">
-        <v>162</v>
+        <v>241</v>
       </c>
     </row>
     <row r="11" spans="1:21" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -2001,7 +2005,7 @@
       </c>
       <c r="F11" s="9"/>
       <c r="G11" s="16" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="H11" s="18">
         <v>8</v>
@@ -2010,7 +2014,7 @@
         <v>20</v>
       </c>
       <c r="J11" s="17" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="K11" s="7" t="s">
         <v>20</v>
@@ -2030,16 +2034,16 @@
         <v>6</v>
       </c>
       <c r="R11" s="11" t="s">
+        <v>162</v>
+      </c>
+      <c r="S11" s="10" t="s">
         <v>163</v>
       </c>
-      <c r="S11" s="10" t="s">
-        <v>164</v>
-      </c>
       <c r="T11" s="12" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="U11" s="10" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="12" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
@@ -2137,7 +2141,7 @@
         <v>20</v>
       </c>
       <c r="J14" s="17" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="K14" s="7" t="s">
         <v>20</v>
@@ -2157,16 +2161,16 @@
         <v>6</v>
       </c>
       <c r="R14" s="11" t="s">
+        <v>162</v>
+      </c>
+      <c r="S14" s="10" t="s">
         <v>163</v>
       </c>
-      <c r="S14" s="10" t="s">
-        <v>164</v>
-      </c>
       <c r="T14" s="12" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="U14" s="10" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="15" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
@@ -2182,12 +2186,10 @@
       <c r="D15" s="15" t="s">
         <v>131</v>
       </c>
-      <c r="E15" s="13" t="s">
-        <v>132</v>
-      </c>
+      <c r="E15" s="13"/>
       <c r="F15" s="9"/>
       <c r="G15" s="16" t="s">
-        <v>182</v>
+        <v>243</v>
       </c>
       <c r="H15" s="18">
         <v>10</v>
@@ -2196,16 +2198,16 @@
         <v>19</v>
       </c>
       <c r="J15" s="17" t="s">
-        <v>183</v>
+        <v>244</v>
       </c>
       <c r="K15" s="7" t="s">
         <v>20</v>
       </c>
       <c r="L15" s="6" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="M15" s="8" t="s">
-        <v>118</v>
+        <v>57</v>
       </c>
       <c r="N15" s="8"/>
       <c r="O15" s="9"/>
@@ -2216,16 +2218,16 @@
         <v>6</v>
       </c>
       <c r="R15" s="11" t="s">
-        <v>163</v>
+        <v>158</v>
       </c>
       <c r="S15" s="10" t="s">
-        <v>184</v>
+        <v>159</v>
       </c>
       <c r="T15" s="12" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
       <c r="U15" s="10" t="s">
-        <v>186</v>
+        <v>161</v>
       </c>
     </row>
     <row r="16" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
@@ -2242,7 +2244,7 @@
         <v>131</v>
       </c>
       <c r="E16" s="13" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="F16" s="9"/>
       <c r="G16" s="16"/>
@@ -2278,47 +2280,21 @@
         <v>133</v>
       </c>
       <c r="F17" s="9"/>
-      <c r="G17" s="16" t="s">
-        <v>192</v>
-      </c>
-      <c r="H17" s="18">
-        <v>11</v>
-      </c>
-      <c r="I17" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="J17" s="17" t="s">
-        <v>193</v>
-      </c>
-      <c r="K17" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="L17" s="6" t="s">
-        <v>8</v>
-      </c>
+      <c r="G17" s="16"/>
+      <c r="H17" s="18"/>
+      <c r="I17" s="5"/>
+      <c r="J17" s="17"/>
+      <c r="K17" s="7"/>
+      <c r="L17" s="6"/>
       <c r="M17" s="8"/>
-      <c r="N17" s="8" t="s">
-        <v>25</v>
-      </c>
+      <c r="N17" s="8"/>
       <c r="O17" s="9"/>
-      <c r="P17" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="Q17" s="10">
-        <v>6</v>
-      </c>
-      <c r="R17" s="11" t="s">
-        <v>163</v>
-      </c>
-      <c r="S17" s="10" t="s">
-        <v>164</v>
-      </c>
-      <c r="T17" s="12" t="s">
-        <v>194</v>
-      </c>
-      <c r="U17" s="10" t="s">
-        <v>166</v>
-      </c>
+      <c r="P17" s="9"/>
+      <c r="Q17" s="10"/>
+      <c r="R17" s="11"/>
+      <c r="S17" s="10"/>
+      <c r="T17" s="12"/>
+      <c r="U17" s="10"/>
     </row>
     <row r="18" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A18" s="4" t="s">
@@ -2338,16 +2314,16 @@
       </c>
       <c r="F18" s="9"/>
       <c r="G18" s="16" t="s">
-        <v>195</v>
+        <v>186</v>
       </c>
       <c r="H18" s="18">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="I18" s="5" t="s">
         <v>20</v>
       </c>
       <c r="J18" s="17" t="s">
-        <v>196</v>
+        <v>187</v>
       </c>
       <c r="K18" s="7" t="s">
         <v>20</v>
@@ -2357,26 +2333,26 @@
       </c>
       <c r="M18" s="8"/>
       <c r="N18" s="8" t="s">
-        <v>43</v>
+        <v>25</v>
       </c>
       <c r="O18" s="9"/>
       <c r="P18" s="9" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="Q18" s="10">
         <v>6</v>
       </c>
       <c r="R18" s="11" t="s">
+        <v>162</v>
+      </c>
+      <c r="S18" s="10" t="s">
         <v>163</v>
       </c>
-      <c r="S18" s="10" t="s">
-        <v>164</v>
-      </c>
       <c r="T18" s="12" t="s">
-        <v>201</v>
+        <v>188</v>
       </c>
       <c r="U18" s="10" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="19" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
@@ -2393,26 +2369,50 @@
         <v>131</v>
       </c>
       <c r="E19" s="13" t="s">
-        <v>134</v>
-      </c>
-      <c r="F19" s="9" t="s">
-        <v>145</v>
-      </c>
-      <c r="G19" s="16"/>
-      <c r="H19" s="18"/>
-      <c r="I19" s="5"/>
-      <c r="J19" s="17"/>
-      <c r="K19" s="7"/>
-      <c r="L19" s="6"/>
+        <v>133</v>
+      </c>
+      <c r="F19" s="9"/>
+      <c r="G19" s="16" t="s">
+        <v>189</v>
+      </c>
+      <c r="H19" s="18">
+        <v>12</v>
+      </c>
+      <c r="I19" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="J19" s="17" t="s">
+        <v>190</v>
+      </c>
+      <c r="K19" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="L19" s="6" t="s">
+        <v>8</v>
+      </c>
       <c r="M19" s="8"/>
-      <c r="N19" s="8"/>
+      <c r="N19" s="8" t="s">
+        <v>43</v>
+      </c>
       <c r="O19" s="9"/>
-      <c r="P19" s="9"/>
-      <c r="Q19" s="10"/>
-      <c r="R19" s="11"/>
-      <c r="S19" s="10"/>
-      <c r="T19" s="12"/>
-      <c r="U19" s="10"/>
+      <c r="P19" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q19" s="10">
+        <v>6</v>
+      </c>
+      <c r="R19" s="11" t="s">
+        <v>162</v>
+      </c>
+      <c r="S19" s="10" t="s">
+        <v>163</v>
+      </c>
+      <c r="T19" s="12" t="s">
+        <v>195</v>
+      </c>
+      <c r="U19" s="10" t="s">
+        <v>165</v>
+      </c>
     </row>
     <row r="20" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A20" s="4" t="s">
@@ -2430,11 +2430,9 @@
       <c r="E20" s="13" t="s">
         <v>134</v>
       </c>
-      <c r="F20" s="9" t="s">
-        <v>146</v>
-      </c>
+      <c r="F20" s="9"/>
       <c r="G20" s="16" t="s">
-        <v>151</v>
+        <v>246</v>
       </c>
       <c r="H20" s="18">
         <v>13</v>
@@ -2443,7 +2441,7 @@
         <v>19</v>
       </c>
       <c r="J20" s="17" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="K20" s="7" t="s">
         <v>20</v>
@@ -2463,16 +2461,16 @@
         <v>6</v>
       </c>
       <c r="R20" s="11" t="s">
+        <v>158</v>
+      </c>
+      <c r="S20" s="10" t="s">
         <v>159</v>
       </c>
-      <c r="S20" s="10" t="s">
-        <v>160</v>
-      </c>
       <c r="T20" s="12" t="s">
-        <v>187</v>
+        <v>245</v>
       </c>
       <c r="U20" s="10" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="21" spans="1:21" ht="45" x14ac:dyDescent="0.25">
@@ -2492,10 +2490,10 @@
         <v>134</v>
       </c>
       <c r="F21" s="9" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="G21" s="16" t="s">
-        <v>188</v>
+        <v>182</v>
       </c>
       <c r="H21" s="18">
         <v>14</v>
@@ -2504,7 +2502,7 @@
         <v>20</v>
       </c>
       <c r="J21" s="17" t="s">
-        <v>189</v>
+        <v>183</v>
       </c>
       <c r="K21" s="7" t="s">
         <v>20</v>
@@ -2517,7 +2515,7 @@
         <v>34</v>
       </c>
       <c r="O21" s="28" t="s">
-        <v>200</v>
+        <v>194</v>
       </c>
       <c r="P21" s="9" t="s">
         <v>19</v>
@@ -2526,16 +2524,16 @@
         <v>6</v>
       </c>
       <c r="R21" s="11" t="s">
+        <v>162</v>
+      </c>
+      <c r="S21" s="10" t="s">
         <v>163</v>
       </c>
-      <c r="S21" s="10" t="s">
-        <v>164</v>
-      </c>
       <c r="T21" s="12" t="s">
-        <v>191</v>
+        <v>185</v>
       </c>
       <c r="U21" s="10" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="22" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
@@ -2558,7 +2556,7 @@
         <v>146</v>
       </c>
       <c r="G22" s="16" t="s">
-        <v>214</v>
+        <v>207</v>
       </c>
       <c r="H22" s="18">
         <v>15</v>
@@ -2567,7 +2565,7 @@
         <v>20</v>
       </c>
       <c r="J22" s="17" t="s">
-        <v>215</v>
+        <v>208</v>
       </c>
       <c r="K22" s="7" t="s">
         <v>20</v>
@@ -2587,16 +2585,16 @@
         <v>6</v>
       </c>
       <c r="R22" s="11" t="s">
+        <v>162</v>
+      </c>
+      <c r="S22" s="10" t="s">
         <v>163</v>
       </c>
-      <c r="S22" s="10" t="s">
-        <v>164</v>
-      </c>
       <c r="T22" s="12" t="s">
-        <v>222</v>
+        <v>215</v>
       </c>
       <c r="U22" s="10" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="23" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
@@ -2617,7 +2615,7 @@
       </c>
       <c r="F23" s="9"/>
       <c r="G23" s="16" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="H23" s="18">
         <v>16</v>
@@ -2626,7 +2624,7 @@
         <v>20</v>
       </c>
       <c r="J23" s="17" t="s">
-        <v>224</v>
+        <v>217</v>
       </c>
       <c r="K23" s="7" t="s">
         <v>20</v>
@@ -2646,16 +2644,16 @@
         <v>6</v>
       </c>
       <c r="R23" s="11" t="s">
+        <v>162</v>
+      </c>
+      <c r="S23" s="10" t="s">
         <v>163</v>
       </c>
-      <c r="S23" s="10" t="s">
-        <v>164</v>
-      </c>
       <c r="T23" s="12" t="s">
-        <v>225</v>
+        <v>218</v>
       </c>
       <c r="U23" s="10" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="24" spans="1:21" ht="30" x14ac:dyDescent="0.25">
@@ -2671,12 +2669,10 @@
       <c r="D24" s="15" t="s">
         <v>136</v>
       </c>
-      <c r="E24" s="13" t="s">
-        <v>137</v>
-      </c>
+      <c r="E24" s="13"/>
       <c r="F24" s="9"/>
       <c r="G24" s="16" t="s">
-        <v>203</v>
+        <v>197</v>
       </c>
       <c r="H24" s="18">
         <v>17</v>
@@ -2685,7 +2681,7 @@
         <v>19</v>
       </c>
       <c r="J24" s="27" t="s">
-        <v>204</v>
+        <v>198</v>
       </c>
       <c r="K24" s="7" t="s">
         <v>20</v>
@@ -2705,16 +2701,16 @@
         <v>6</v>
       </c>
       <c r="R24" s="11" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="S24" s="10" t="s">
-        <v>184</v>
+        <v>179</v>
       </c>
       <c r="T24" s="12" t="s">
-        <v>205</v>
+        <v>199</v>
       </c>
       <c r="U24" s="10" t="s">
-        <v>186</v>
+        <v>180</v>
       </c>
     </row>
     <row r="25" spans="1:21" ht="45" x14ac:dyDescent="0.25">
@@ -2735,7 +2731,7 @@
       </c>
       <c r="F25" s="9"/>
       <c r="G25" s="16" t="s">
-        <v>245</v>
+        <v>238</v>
       </c>
       <c r="H25" s="18">
         <v>18</v>
@@ -2744,7 +2740,7 @@
         <v>20</v>
       </c>
       <c r="J25" s="27" t="s">
-        <v>230</v>
+        <v>223</v>
       </c>
       <c r="K25" s="7" t="s">
         <v>20</v>
@@ -2757,7 +2753,7 @@
         <v>34</v>
       </c>
       <c r="O25" s="28" t="s">
-        <v>209</v>
+        <v>202</v>
       </c>
       <c r="P25" s="9" t="s">
         <v>19</v>
@@ -2766,16 +2762,16 @@
         <v>6</v>
       </c>
       <c r="R25" s="11" t="s">
+        <v>162</v>
+      </c>
+      <c r="S25" s="10" t="s">
         <v>163</v>
       </c>
-      <c r="S25" s="10" t="s">
-        <v>164</v>
-      </c>
       <c r="T25" s="12" t="s">
-        <v>210</v>
+        <v>203</v>
       </c>
       <c r="U25" s="10" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="26" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
@@ -2796,7 +2792,7 @@
       </c>
       <c r="F26" s="9"/>
       <c r="G26" s="16" t="s">
-        <v>213</v>
+        <v>206</v>
       </c>
       <c r="H26" s="18">
         <v>19</v>
@@ -2805,7 +2801,7 @@
         <v>20</v>
       </c>
       <c r="J26" s="27" t="s">
-        <v>211</v>
+        <v>204</v>
       </c>
       <c r="K26" s="7" t="s">
         <v>20</v>
@@ -2825,16 +2821,16 @@
         <v>6</v>
       </c>
       <c r="R26" s="11" t="s">
+        <v>162</v>
+      </c>
+      <c r="S26" s="10" t="s">
         <v>163</v>
       </c>
-      <c r="S26" s="10" t="s">
-        <v>164</v>
-      </c>
       <c r="T26" s="12" t="s">
-        <v>212</v>
+        <v>205</v>
       </c>
       <c r="U26" s="10" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="27" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
@@ -2892,7 +2888,7 @@
         <v>148</v>
       </c>
       <c r="G28" s="16" t="s">
-        <v>216</v>
+        <v>209</v>
       </c>
       <c r="H28" s="18">
         <v>20</v>
@@ -2901,7 +2897,7 @@
         <v>20</v>
       </c>
       <c r="J28" s="27" t="s">
-        <v>219</v>
+        <v>212</v>
       </c>
       <c r="K28" s="7" t="s">
         <v>20</v>
@@ -2914,7 +2910,7 @@
         <v>34</v>
       </c>
       <c r="O28" s="28" t="s">
-        <v>217</v>
+        <v>210</v>
       </c>
       <c r="P28" s="9" t="s">
         <v>19</v>
@@ -2923,16 +2919,16 @@
         <v>6</v>
       </c>
       <c r="R28" s="11" t="s">
+        <v>162</v>
+      </c>
+      <c r="S28" s="10" t="s">
         <v>163</v>
       </c>
-      <c r="S28" s="10" t="s">
-        <v>164</v>
-      </c>
       <c r="T28" s="12" t="s">
-        <v>218</v>
+        <v>211</v>
       </c>
       <c r="U28" s="10" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="29" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
@@ -2953,7 +2949,7 @@
       </c>
       <c r="F29" s="9"/>
       <c r="G29" s="16" t="s">
-        <v>206</v>
+        <v>247</v>
       </c>
       <c r="H29" s="18">
         <v>21</v>
@@ -2962,7 +2958,7 @@
         <v>19</v>
       </c>
       <c r="J29" s="27" t="s">
-        <v>207</v>
+        <v>200</v>
       </c>
       <c r="K29" s="7" t="s">
         <v>20</v>
@@ -2982,16 +2978,16 @@
         <v>6</v>
       </c>
       <c r="R29" s="11" t="s">
+        <v>158</v>
+      </c>
+      <c r="S29" s="10" t="s">
         <v>159</v>
       </c>
-      <c r="S29" s="10" t="s">
-        <v>160</v>
-      </c>
       <c r="T29" s="12" t="s">
-        <v>208</v>
+        <v>201</v>
       </c>
       <c r="U29" s="10" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="30" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
@@ -3012,7 +3008,7 @@
       </c>
       <c r="F30" s="9"/>
       <c r="G30" s="16" t="s">
-        <v>220</v>
+        <v>213</v>
       </c>
       <c r="H30" s="18">
         <v>22</v>
@@ -3021,7 +3017,7 @@
         <v>20</v>
       </c>
       <c r="J30" s="27" t="s">
-        <v>221</v>
+        <v>214</v>
       </c>
       <c r="K30" s="7" t="s">
         <v>20</v>
@@ -3041,16 +3037,16 @@
         <v>6</v>
       </c>
       <c r="R30" s="11" t="s">
+        <v>162</v>
+      </c>
+      <c r="S30" s="10" t="s">
         <v>163</v>
       </c>
-      <c r="S30" s="10" t="s">
-        <v>164</v>
-      </c>
       <c r="T30" s="12" t="s">
-        <v>223</v>
+        <v>216</v>
       </c>
       <c r="U30" s="10" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="31" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
@@ -3071,7 +3067,7 @@
       </c>
       <c r="F31" s="9"/>
       <c r="G31" s="16" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="H31" s="18">
         <v>23</v>
@@ -3080,7 +3076,7 @@
         <v>20</v>
       </c>
       <c r="J31" s="17" t="s">
-        <v>226</v>
+        <v>219</v>
       </c>
       <c r="K31" s="7" t="s">
         <v>20</v>
@@ -3100,16 +3096,16 @@
         <v>6</v>
       </c>
       <c r="R31" s="11" t="s">
+        <v>162</v>
+      </c>
+      <c r="S31" s="10" t="s">
         <v>163</v>
       </c>
-      <c r="S31" s="10" t="s">
-        <v>164</v>
-      </c>
       <c r="T31" s="12" t="s">
-        <v>227</v>
+        <v>220</v>
       </c>
       <c r="U31" s="10" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="32" spans="1:21" ht="30" x14ac:dyDescent="0.25">
@@ -3128,7 +3124,7 @@
       <c r="E32" s="13"/>
       <c r="F32" s="9"/>
       <c r="G32" s="29" t="s">
-        <v>239</v>
+        <v>232</v>
       </c>
       <c r="H32" s="18">
         <v>24</v>
@@ -3137,7 +3133,7 @@
         <v>20</v>
       </c>
       <c r="J32" s="27" t="s">
-        <v>231</v>
+        <v>224</v>
       </c>
       <c r="K32" s="7" t="s">
         <v>20</v>
@@ -3157,16 +3153,16 @@
         <v>6</v>
       </c>
       <c r="R32" s="11" t="s">
+        <v>162</v>
+      </c>
+      <c r="S32" s="10" t="s">
         <v>163</v>
       </c>
-      <c r="S32" s="10" t="s">
-        <v>164</v>
-      </c>
       <c r="T32" s="12" t="s">
-        <v>232</v>
+        <v>225</v>
       </c>
       <c r="U32" s="10" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="33" spans="1:21" ht="30" x14ac:dyDescent="0.25">
@@ -3185,7 +3181,7 @@
       <c r="E33" s="13"/>
       <c r="F33" s="9"/>
       <c r="G33" s="29" t="s">
-        <v>233</v>
+        <v>226</v>
       </c>
       <c r="H33" s="18">
         <v>25</v>
@@ -3194,7 +3190,7 @@
         <v>20</v>
       </c>
       <c r="J33" s="27" t="s">
-        <v>234</v>
+        <v>227</v>
       </c>
       <c r="K33" s="7" t="s">
         <v>20</v>
@@ -3214,16 +3210,16 @@
         <v>6</v>
       </c>
       <c r="R33" s="11" t="s">
+        <v>162</v>
+      </c>
+      <c r="S33" s="10" t="s">
         <v>163</v>
       </c>
-      <c r="S33" s="10" t="s">
-        <v>164</v>
-      </c>
       <c r="T33" s="12" t="s">
-        <v>235</v>
+        <v>228</v>
       </c>
       <c r="U33" s="10" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="34" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
@@ -3237,7 +3233,7 @@
         <v>123</v>
       </c>
       <c r="D34" s="15" t="s">
-        <v>236</v>
+        <v>229</v>
       </c>
       <c r="E34" s="13"/>
       <c r="F34" s="9"/>
@@ -3251,7 +3247,7 @@
         <v>20</v>
       </c>
       <c r="J34" s="17" t="s">
-        <v>237</v>
+        <v>230</v>
       </c>
       <c r="K34" s="7" t="s">
         <v>20</v>
@@ -3282,12 +3278,12 @@
         <v>123</v>
       </c>
       <c r="D35" s="15" t="s">
-        <v>236</v>
+        <v>229</v>
       </c>
       <c r="E35" s="13"/>
       <c r="F35" s="9"/>
       <c r="G35" s="16" t="s">
-        <v>238</v>
+        <v>231</v>
       </c>
       <c r="H35" s="18">
         <v>27</v>
@@ -3296,7 +3292,7 @@
         <v>20</v>
       </c>
       <c r="J35" s="17" t="s">
-        <v>240</v>
+        <v>233</v>
       </c>
       <c r="K35" s="7" t="s">
         <v>20</v>
@@ -3316,16 +3312,16 @@
         <v>6</v>
       </c>
       <c r="R35" s="11" t="s">
+        <v>162</v>
+      </c>
+      <c r="S35" s="10" t="s">
         <v>163</v>
       </c>
-      <c r="S35" s="10" t="s">
-        <v>164</v>
-      </c>
       <c r="T35" s="12" t="s">
-        <v>241</v>
+        <v>234</v>
       </c>
       <c r="U35" s="10" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="36" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
@@ -3342,7 +3338,7 @@
       <c r="E36" s="13"/>
       <c r="F36" s="9"/>
       <c r="G36" s="16" t="s">
-        <v>242</v>
+        <v>235</v>
       </c>
       <c r="H36" s="18">
         <v>28</v>
@@ -3351,7 +3347,7 @@
         <v>20</v>
       </c>
       <c r="J36" s="17" t="s">
-        <v>244</v>
+        <v>237</v>
       </c>
       <c r="K36" s="7" t="s">
         <v>20</v>
@@ -3371,16 +3367,16 @@
         <v>6</v>
       </c>
       <c r="R36" s="11" t="s">
+        <v>162</v>
+      </c>
+      <c r="S36" s="10" t="s">
         <v>163</v>
       </c>
-      <c r="S36" s="10" t="s">
-        <v>164</v>
-      </c>
       <c r="T36" s="12" t="s">
-        <v>243</v>
+        <v>236</v>
       </c>
       <c r="U36" s="10" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="37" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
@@ -4711,10 +4707,16 @@
     <row r="291" hidden="1" x14ac:dyDescent="0.25"/>
     <row r="292" hidden="1" x14ac:dyDescent="0.25"/>
   </sheetData>
-  <autoFilter ref="A1:U32">
+  <autoFilter ref="A1:U36">
     <filterColumn colId="12" showButton="0"/>
   </autoFilter>
   <mergeCells count="20">
+    <mergeCell ref="P1:P2"/>
+    <mergeCell ref="U1:U2"/>
+    <mergeCell ref="T1:T2"/>
+    <mergeCell ref="S1:S2"/>
+    <mergeCell ref="R1:R2"/>
+    <mergeCell ref="Q1:Q2"/>
     <mergeCell ref="I1:I2"/>
     <mergeCell ref="H1:H2"/>
     <mergeCell ref="O1:O2"/>
@@ -4729,19 +4731,13 @@
     <mergeCell ref="D1:D2"/>
     <mergeCell ref="C1:C2"/>
     <mergeCell ref="F1:F2"/>
-    <mergeCell ref="P1:P2"/>
-    <mergeCell ref="U1:U2"/>
-    <mergeCell ref="T1:T2"/>
-    <mergeCell ref="S1:S2"/>
-    <mergeCell ref="R1:R2"/>
-    <mergeCell ref="Q1:Q2"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="O21" r:id="rId1"/>
-    <hyperlink ref="O10" r:id="rId2"/>
-    <hyperlink ref="O7" r:id="rId3"/>
-    <hyperlink ref="O25" r:id="rId4"/>
-    <hyperlink ref="O28" r:id="rId5"/>
+    <hyperlink ref="O10" r:id="rId1"/>
+    <hyperlink ref="O7" r:id="rId2"/>
+    <hyperlink ref="O25" r:id="rId3"/>
+    <hyperlink ref="O28" r:id="rId4"/>
+    <hyperlink ref="O21" r:id="rId5"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId6"/>

</xml_diff>